<commit_message>
New job applications and new June resume
</commit_message>
<xml_diff>
--- a/assets/resume/JobApplications.xlsx
+++ b/assets/resume/JobApplications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\WebstormProjects\MyWebsite2021\assets\resume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD13ED55-6E00-4CA0-BC4C-5C02E57E18DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608DAD37-0E05-42B4-BCE0-36E79C5ADBC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{48A125A1-E177-474A-95CA-3480FD29D6E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
   <si>
     <t>Revature</t>
   </si>
@@ -143,9 +143,6 @@
     <t>https://ea.gr8people.com/jobs/165952/online-software-engineer-fifa?locale=en</t>
   </si>
   <si>
-    <t>Ghost Punch</t>
-  </si>
-  <si>
     <t>https://ghostpunch.freshteam.com/jobs/yj56pIB886GP/ui-engineer</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>Submitted - Rejected</t>
   </si>
   <si>
-    <t>Submitted 5/25/2022 - rejected</t>
-  </si>
-  <si>
     <t>SalesForce</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t>Submitted 6/17/22</t>
   </si>
   <si>
-    <t>Avandale</t>
-  </si>
-  <si>
     <t>Submitted 6/19/22</t>
   </si>
   <si>
@@ -198,16 +189,128 @@
   </si>
   <si>
     <t>Backend Engineer - Personalization</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>JavaScript Full Stack Developer</t>
+  </si>
+  <si>
+    <t>Full Stack Developer</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3106559830?lipi=urn%3Ali%3Apage%3Ad_flagship3_job_details%3BoOlql8b9SR%2B2kCfGpZLNmw%3D%3D</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>Software Engineer Cloud Infra- Slack (SWE II and SWE I levels)</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3119733149?lipi=urn%3Ali%3Apage%3Ad_flagship3_job_details%3BD8eIp96FQFOFlEQnObftpA%3D%3D</t>
+  </si>
+  <si>
+    <t>Dropbox</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/2921313406/</t>
+  </si>
+  <si>
+    <t>SoFi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3125153562/</t>
+  </si>
+  <si>
+    <t>New Grad, Software Development Engineer - Credit Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Engineer - Undergrad New College Grad </t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3118239408/</t>
+  </si>
+  <si>
+    <t>Software Engineer Asc - Entry Level / App SW / DecSecOps / Orlando</t>
+  </si>
+  <si>
+    <t>Lockheed Martin</t>
+  </si>
+  <si>
+    <t>Submitted 6/28/21</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3137759202/</t>
+  </si>
+  <si>
+    <r>
+      <t>Avandale</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (REJECTED)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ghost Punch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(REJECTED)</t>
+    </r>
+  </si>
+  <si>
+    <t>Nightfall AI - Cybersecurity startup</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3137236082/</t>
+  </si>
+  <si>
+    <t>New Grad Backend Engineer (Remote) - US &amp; Canada</t>
+  </si>
+  <si>
+    <t>Software Engineer (Open to remote work, except the following locations: SD, VT, and WV)</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>https://jobs.nike.com/job/00560927</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -646,7 +749,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -681,15 +784,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4007B6-169F-47BF-80A8-4EA96A7D76CA}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
     <col min="2" max="2" width="77.7109375" customWidth="1"/>
     <col min="3" max="3" width="39.5703125" customWidth="1"/>
     <col min="4" max="4" width="97.85546875" customWidth="1"/>
@@ -763,76 +866,203 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
         <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
August additions to job search'
</commit_message>
<xml_diff>
--- a/assets/resume/JobApplications.xlsx
+++ b/assets/resume/JobApplications.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\WebstormProjects\MyWebsite2021\assets\resume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A748608C-1314-4127-8676-AC5F8F4FCD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA11D47B-0701-4BF2-98FA-0E3738D43599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{48A125A1-E177-474A-95CA-3480FD29D6E0}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{48A125A1-E177-474A-95CA-3480FD29D6E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Denver Jobs" sheetId="1" r:id="rId1"/>
     <sheet name="Dream jobs" sheetId="2" r:id="rId2"/>
     <sheet name="Big Companies" sheetId="3" r:id="rId3"/>
+    <sheet name="Interviews" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="135">
   <si>
     <t>Revature</t>
   </si>
@@ -496,12 +497,54 @@
   <si>
     <t>https://www.linkedin.com/safety/go?url=https%3A%2F%2Fcareers.cerner.com%2Fjob%2F91914BR&amp;trk=flagship-messaging-web&amp;messageThreadUrn=urn%3Ali%3AmessagingThread%3A2-NWViOTcwNzgtMDY5My00Njg0LWEzMDctYTgwYzYxMTdlNTQ5XzAxMg%3D%3D&amp;lipi=urn%3Ali%3Apage%3Ad_flagship3_profile_view_base%3B9QZAkTnLQG2a7VBU4%2FgCDg%3D%3D</t>
   </si>
+  <si>
+    <t>Software Engineer, Personalization Application Core</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>Submitted 8/4/22</t>
+  </si>
+  <si>
+    <t>https://jobs.netflix.com/jobs/219156808</t>
+  </si>
+  <si>
+    <t>Enterprise Fleet</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Job Tech Stack</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>71k</t>
+  </si>
+  <si>
+    <t>125k</t>
+  </si>
+  <si>
+    <t>Interview Time</t>
+  </si>
+  <si>
+    <t>Java,Angular,hosted on Oracle</t>
+  </si>
+  <si>
+    <t>How I found</t>
+  </si>
+  <si>
+    <t>Recruiter Linked Reached Out to Me</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,6 +555,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -537,8 +588,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4007B6-169F-47BF-80A8-4EA96A7D76CA}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,6 +1494,87 @@
         <v>120</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D26D90-2AC2-45DA-89C3-A3DBB59CC215}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44782</v>
+      </c>
+      <c r="E2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>